<commit_message>
Yahor-ipusers-password was changed for FSTestUser2
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C796672
</commit_message>
<xml_diff>
--- a/PPIUK-IPUsers/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-IPUsers/src/test/resources/CobaltUsers.xlsx
@@ -864,7 +864,7 @@
     <t>Main FS user</t>
   </si>
   <si>
-    <t>Password123456!</t>
+    <t>Password111!</t>
   </si>
 </sst>
 </file>
@@ -1288,7 +1288,7 @@
   <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>